<commit_message>
dodadeno upatstvo za merge branch
</commit_message>
<xml_diff>
--- a/Project-MRA/Project MRA.xlsx
+++ b/Project-MRA/Project MRA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Desktop\Tenderi\WEB\PROG\Qinshift-homeworks\Project-MRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF882E54-35DA-4B0C-B763-2EBED5A37701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1208F106-7482-4795-974E-3A925CCCAEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="764" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="DB" sheetId="3" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId8"/>
     <sheet name="mraMongoose" sheetId="6" r:id="rId9"/>
-    <sheet name="contactPage" sheetId="5" r:id="rId10"/>
+    <sheet name="Upatstvo" sheetId="5" r:id="rId10"/>
     <sheet name="multilingual" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="812">
   <si>
     <t>Contact details</t>
   </si>
@@ -8374,31 +8374,8 @@
     <t>Upload_preset:unsigned_preset</t>
   </si>
   <si>
-    <t xml:space="preserve">Preimenuvani se klasite </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se izbrisani </t>
-  </si>
-  <si>
-    <t>#languageToggle</t>
-  </si>
-  <si>
-    <t>#dropdownToggle</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">.dorpdown </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vo</t>
+    <r>
+      <t xml:space="preserve">Za integriranje na </t>
     </r>
     <r>
       <rPr>
@@ -8410,12 +8387,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> .dropdownLanguageSelector</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">.dorpdown-toggle </t>
+      <t xml:space="preserve">multilingual </t>
     </r>
     <r>
       <rPr>
@@ -8426,7 +8398,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>vo</t>
+      <t>vo display text od</t>
     </r>
     <r>
       <rPr>
@@ -8438,12 +8410,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> .dropdownLanguageSelector-toggle</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">.dorpdown-menu </t>
+      <t xml:space="preserve"> footer</t>
     </r>
     <r>
       <rPr>
@@ -8454,7 +8421,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>vo</t>
+      <t xml:space="preserve"> od ticket </t>
     </r>
     <r>
       <rPr>
@@ -8466,8 +8433,44 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> .dropdownLanguageSelector-menu</t>
-    </r>
+      <t>Footer#10</t>
+    </r>
+  </si>
+  <si>
+    <t>Vo nego dodadeni se potrebnite klasi kaj site elementi koi prikazuvaat text koj zavisi od izborot na jazik na aplikacijata.</t>
+  </si>
+  <si>
+    <t>Kreiran e main.css koj sodrzi:</t>
+  </si>
+  <si>
+    <t>VAZNO:</t>
+  </si>
+  <si>
+    <t>&lt;head&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;meta charset="UTF-8"&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;meta name="viewport" content="width=device-width, initial-scale=1.0"&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;link rel="stylesheet" href="../css/main.css"&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;link rel="stylesheet" href="https://cdnjs.cloudflare.com/ajax/libs/font-awesome/4.7.0/css/font-awesome.min.css"&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;title&gt;Page&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/head&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;script src="../scripts/main.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;script src="../modules/multilingual.js"&gt;&lt;/script&gt;</t>
   </si>
   <si>
     <r>
@@ -8491,6 +8494,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> vo </t>
@@ -8513,6 +8517,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> od ticket </t>
@@ -8552,6 +8557,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, kopiran e block </t>
@@ -8566,7 +8572,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>nav</t>
+      <t xml:space="preserve">nav </t>
     </r>
     <r>
       <rPr>
@@ -8574,9 +8580,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I vo nego vo poslednoto </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>od</t>
     </r>
     <r>
       <rPr>
@@ -8588,7 +8595,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>li</t>
+      <t xml:space="preserve"> navBar#10</t>
     </r>
     <r>
       <rPr>
@@ -8596,9 +8603,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> celosniot </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I vo nego vo poslednoto </t>
     </r>
     <r>
       <rPr>
@@ -8610,7 +8618,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>div</t>
+      <t>li</t>
     </r>
     <r>
       <rPr>
@@ -8618,14 +8626,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e zamenet so nov.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vo </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> celosniot </t>
     </r>
     <r>
       <rPr>
@@ -8637,7 +8641,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>main.css</t>
+      <t>div</t>
     </r>
     <r>
       <rPr>
@@ -8645,14 +8649,15 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (PREDVIDENO E main.css od navBar#9 da bide konecniot main.css)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Za integriranje na </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e zamenet so nov.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vo celtiot block </t>
     </r>
     <r>
       <rPr>
@@ -8664,7 +8669,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">multilingual </t>
+      <t>nav</t>
     </r>
     <r>
       <rPr>
@@ -8675,7 +8680,12 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>vo display text od</t>
+      <t xml:space="preserve"> se dodadeni se potrebnite klasi kaj site elementi koi prikazuvaat text koj zavisi od izborot na jazik na aplikacijata.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vo </t>
     </r>
     <r>
       <rPr>
@@ -8687,7 +8697,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> footer</t>
+      <t>main.js</t>
     </r>
     <r>
       <rPr>
@@ -8698,7 +8708,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> od ticket </t>
+      <t xml:space="preserve"> e celosno prevzement kodot od </t>
     </r>
     <r>
       <rPr>
@@ -8710,12 +8720,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Footer#10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kodot od </t>
+      <t>main.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> na </t>
     </r>
     <r>
       <rPr>
@@ -8727,7 +8743,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>konecniot</t>
+      <t>navBar#9</t>
     </r>
     <r>
       <rPr>
@@ -8735,9 +8751,15 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Blokot </t>
     </r>
     <r>
       <rPr>
@@ -8749,7 +8771,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>main.css</t>
+      <t>header</t>
     </r>
     <r>
       <rPr>
@@ -8757,9 +8779,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> koj se odnesuva na </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, od </t>
     </r>
     <r>
       <rPr>
@@ -8771,7 +8794,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>footer</t>
+      <t>contact.html</t>
     </r>
     <r>
       <rPr>
@@ -8779,9 +8802,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, e zamenet so celosniot kod od </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e spremen da se kopira vo site preostanati .</t>
     </r>
     <r>
       <rPr>
@@ -8793,7 +8817,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">main.css </t>
+      <t>html</t>
     </r>
     <r>
       <rPr>
@@ -8801,9 +8825,15 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">od tiket  </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> strani.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Celosniot kod za </t>
     </r>
     <r>
       <rPr>
@@ -8815,12 +8845,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Footer#10 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Celosniot kod za </t>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> od </t>
     </r>
     <r>
       <rPr>
@@ -8832,7 +8868,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>footer</t>
+      <t>Footer#10</t>
     </r>
     <r>
       <rPr>
@@ -8840,9 +8876,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> od </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e staven kako </t>
     </r>
     <r>
       <rPr>
@@ -8854,7 +8891,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Footer#10</t>
+      <t>footer</t>
     </r>
     <r>
       <rPr>
@@ -8862,9 +8899,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e staven kako </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vo </t>
     </r>
     <r>
       <rPr>
@@ -8876,17 +8914,12 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>footer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> vo </t>
+      <t>contact.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Blokot </t>
     </r>
     <r>
       <rPr>
@@ -8898,15 +8931,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>contact.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Dodadeni se potrebnite klasi kaj site elementi koi prikazuvaat text koj zavisi od izborot na jazik na aplikacijata.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Blokot </t>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, od </t>
     </r>
     <r>
       <rPr>
@@ -8918,7 +8954,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>footer</t>
+      <t>contact.html</t>
     </r>
     <r>
       <rPr>
@@ -8926,9 +8962,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, od </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e spremen da se kopira vo site preostanati .</t>
     </r>
     <r>
       <rPr>
@@ -8940,7 +8977,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>contact.html</t>
+      <t>html</t>
     </r>
     <r>
       <rPr>
@@ -8948,9 +8985,15 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e spremen da se kopira vo site preostanati .</t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> strani.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">blok namenet za </t>
     </r>
     <r>
       <rPr>
@@ -8962,7 +9005,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>html</t>
+      <t>footer</t>
     </r>
     <r>
       <rPr>
@@ -8970,14 +9013,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> strani.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Blokot </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, prevzemen kompletno od ticket </t>
     </r>
     <r>
       <rPr>
@@ -8989,7 +9028,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>header</t>
+      <t>Footer#10</t>
     </r>
     <r>
       <rPr>
@@ -8997,9 +9036,15 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, od </t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> so napraveni minimalni korekcii vo pozicioniranje I otstraneti nepostoecki klasi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">blok namenet za </t>
     </r>
     <r>
       <rPr>
@@ -9011,7 +9056,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>contact.html</t>
+      <t>header</t>
     </r>
     <r>
       <rPr>
@@ -9019,9 +9064,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e spremen da se kopira vo site preostanati .</t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, prevzemen od ticket </t>
     </r>
     <r>
       <rPr>
@@ -9033,7 +9079,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>html</t>
+      <t>navBar#9</t>
     </r>
     <r>
       <rPr>
@@ -9041,9 +9087,496 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> strani.</t>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, so promena vo delot koj se odnesuva na </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>language selector dropdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Koga vo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">main.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ili </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se dodava kod treba, pocetokot I krajot na noviot kod, so komentiranje da se oznaci na sto se odnesuva… </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Za da kodot se loadira po pravilen redosled I se da funkcionira treba, koga se integriraat </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file-ovite da bidat na sledniot nacin:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">najgore vo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;head&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> da bidat .css po sledniot redosled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>  &lt;link rel="stylesheet" href="../css/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.css"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">najdolu pred </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/body&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>da bidat .js po sledniot redosled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>  &lt;script src="../scripts/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.js"&gt;&lt;/script&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Koga treba da se stavaat kartickite koi kje se renderiraat na </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>services.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, treba tie da se kreiraat vo stranata </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contact.html</t>
+    </r>
+  </si>
+  <si>
+    <t>4. Koga nekoj tekst treba da se prikaze na ekran preku nekoj element mora:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">toj element da ima klasi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">onscreenText pagenamehtmlUniquename </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tekstot koj treba da se prikaze ne se pisuva pomegju otvoracki I zatvaracki </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tag </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>na toj element</t>
+    </r>
+  </si>
+  <si>
+    <t>Primer:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tekstot koj treba da se prikaze treba da se prevede na germanski, angliski I makedonski I istiot direktno da se vnese vo file-ot </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contents.json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folderot</t>
+    </r>
+  </si>
+  <si>
+    <t>  {</t>
+  </si>
+  <si>
+    <t>  }</t>
+  </si>
+  <si>
+    <t>    "id": "homepagehtmlHome",</t>
+  </si>
+  <si>
+    <t>    "english": "Home",</t>
+  </si>
+  <si>
+    <t>    "macedonian": "Дома"</t>
+  </si>
+  <si>
+    <t>    "german": "Heim",</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ako treba na homePage.html preku </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p tag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> da se ispise tekst "Home", treba: </t>
+    </r>
+  </si>
+  <si>
+    <t>Da se vpise     &lt;p class="onscreenText homepagehtmlHome"&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Namesto      </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;p&gt;Home&lt;/p&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contents.json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> da se dodade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Strukturata na branch-ata e MVC patern, odnosno, za da se testira otkako kje se merge-ne, prvo treba da se izvrsi npm install, potoa npm run dev, i se pristapuva preku API so </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://localhost:3000/pagename.html</t>
     </r>
   </si>
 </sst>
@@ -9051,7 +9584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42">
+  <fonts count="47">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9341,6 +9874,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -9382,7 +9952,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -9500,7 +10070,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -9522,6 +10091,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13537,96 +14114,251 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B3:E19"/>
+  <dimension ref="B2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="49"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:5">
-      <c r="B3" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" s="49" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="C3" s="49" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="D4" s="49" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="C5" s="49" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="C6" s="49" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="49" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="C9" s="49" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="D10" s="49" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="C11" s="49" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="49" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="C15" s="49" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" s="49" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="49" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" s="49" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" s="49" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="D21" s="49" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="E22" s="50" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="E23" s="50" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="E24" s="50" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="E25" s="50" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="E26" s="50" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="C4" t="s">
+    <row r="27" spans="2:5">
+      <c r="E27" s="50" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="E28" s="50" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="C5" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="D6" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="E7" s="41" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="E8" s="41" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="D9" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="E10" s="41" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="E11" s="41" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="E12" s="41" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" t="s">
+    <row r="29" spans="2:5">
+      <c r="E29" s="50" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
-      <c r="C16" t="s">
+    <row r="30" spans="2:5">
+      <c r="D30" s="49" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="E31" s="50" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="E32" s="50" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="E33" s="50" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
-      <c r="D17" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19" t="s">
-        <v>781</v>
+    <row r="34" spans="3:7">
+      <c r="E34" s="50" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="49" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="49" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="D37" s="49" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="D38" s="49" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="D39" s="49" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="D40" s="51" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="E41" s="49" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="F42" s="49" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="F43" s="49" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="F44" s="49" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="G45" s="48" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="G46" s="48" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="G47" s="48" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="G48" s="48" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="G49" s="48" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7">
+      <c r="G50" s="48" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" s="49" t="s">
+        <v>811</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13647,59 +14379,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>357</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>358</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>359</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>360</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>361</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
@@ -13718,11 +14450,11 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6"/>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>363</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
     </row>
     <row r="11" spans="1:4" ht="45">
       <c r="A11" s="6"/>
@@ -13759,10 +14491,10 @@
     <row r="15" spans="1:4">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="47" t="s">
         <v>368</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="47"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
@@ -14374,140 +15106,140 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="127.5">
-      <c r="A117" s="42" t="s">
+      <c r="A117" s="41" t="s">
         <v>537</v>
       </c>
       <c r="B117" s="21" t="s">
         <v>538</v>
       </c>
-      <c r="C117" s="45" t="s">
+      <c r="C117" s="44" t="s">
         <v>542</v>
       </c>
-      <c r="D117" s="45" t="s">
+      <c r="D117" s="44" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="25.5">
-      <c r="A118" s="43"/>
+      <c r="A118" s="42"/>
       <c r="B118" s="21" t="s">
         <v>539</v>
       </c>
-      <c r="C118" s="46"/>
-      <c r="D118" s="46"/>
+      <c r="C118" s="45"/>
+      <c r="D118" s="45"/>
     </row>
     <row r="119" spans="1:4" ht="51">
-      <c r="A119" s="43"/>
+      <c r="A119" s="42"/>
       <c r="B119" s="21" t="s">
         <v>540</v>
       </c>
-      <c r="C119" s="46"/>
-      <c r="D119" s="46"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="45"/>
     </row>
     <row r="120" spans="1:4" ht="51.75" thickBot="1">
-      <c r="A120" s="44"/>
+      <c r="A120" s="43"/>
       <c r="B120" s="22" t="s">
         <v>541</v>
       </c>
-      <c r="C120" s="47"/>
-      <c r="D120" s="47"/>
+      <c r="C120" s="46"/>
+      <c r="D120" s="46"/>
     </row>
     <row r="121" spans="1:4" ht="38.25">
-      <c r="A121" s="42" t="s">
+      <c r="A121" s="41" t="s">
         <v>544</v>
       </c>
       <c r="B121" s="21" t="s">
         <v>545</v>
       </c>
-      <c r="C121" s="45" t="s">
+      <c r="C121" s="44" t="s">
         <v>549</v>
       </c>
-      <c r="D121" s="45" t="s">
+      <c r="D121" s="44" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="25.5">
-      <c r="A122" s="43"/>
+      <c r="A122" s="42"/>
       <c r="B122" s="21" t="s">
         <v>546</v>
       </c>
-      <c r="C122" s="46"/>
-      <c r="D122" s="46"/>
+      <c r="C122" s="45"/>
+      <c r="D122" s="45"/>
     </row>
     <row r="123" spans="1:4" ht="51">
-      <c r="A123" s="43"/>
+      <c r="A123" s="42"/>
       <c r="B123" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="C123" s="46"/>
-      <c r="D123" s="46"/>
+      <c r="C123" s="45"/>
+      <c r="D123" s="45"/>
     </row>
     <row r="124" spans="1:4" ht="26.25" thickBot="1">
-      <c r="A124" s="44"/>
+      <c r="A124" s="43"/>
       <c r="B124" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="C124" s="47"/>
-      <c r="D124" s="47"/>
+      <c r="C124" s="46"/>
+      <c r="D124" s="46"/>
     </row>
     <row r="125" spans="1:4" ht="38.25">
-      <c r="A125" s="42" t="s">
+      <c r="A125" s="41" t="s">
         <v>551</v>
       </c>
       <c r="B125" s="21" t="s">
         <v>552</v>
       </c>
-      <c r="C125" s="45" t="s">
+      <c r="C125" s="44" t="s">
         <v>555</v>
       </c>
-      <c r="D125" s="45" t="s">
+      <c r="D125" s="44" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="63.75">
-      <c r="A126" s="43"/>
+      <c r="A126" s="42"/>
       <c r="B126" s="21" t="s">
         <v>553</v>
       </c>
-      <c r="C126" s="46"/>
-      <c r="D126" s="46"/>
+      <c r="C126" s="45"/>
+      <c r="D126" s="45"/>
     </row>
     <row r="127" spans="1:4" ht="90" thickBot="1">
-      <c r="A127" s="44"/>
+      <c r="A127" s="43"/>
       <c r="B127" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="C127" s="47"/>
-      <c r="D127" s="47"/>
+      <c r="C127" s="46"/>
+      <c r="D127" s="46"/>
     </row>
     <row r="128" spans="1:4" ht="51">
-      <c r="A128" s="42" t="s">
+      <c r="A128" s="41" t="s">
         <v>557</v>
       </c>
       <c r="B128" s="21" t="s">
         <v>558</v>
       </c>
-      <c r="C128" s="45" t="s">
+      <c r="C128" s="44" t="s">
         <v>561</v>
       </c>
-      <c r="D128" s="45" t="s">
+      <c r="D128" s="44" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="38.25">
-      <c r="A129" s="43"/>
+      <c r="A129" s="42"/>
       <c r="B129" s="21" t="s">
         <v>559</v>
       </c>
-      <c r="C129" s="46"/>
-      <c r="D129" s="46"/>
+      <c r="C129" s="45"/>
+      <c r="D129" s="45"/>
     </row>
     <row r="130" spans="1:4" ht="51">
-      <c r="A130" s="43"/>
+      <c r="A130" s="42"/>
       <c r="B130" s="21" t="s">
         <v>560</v>
       </c>
-      <c r="C130" s="46"/>
-      <c r="D130" s="46"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="6"/>
@@ -16291,18 +17023,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="D117:D120"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="D121:D124"/>
     <mergeCell ref="A125:A127"/>
     <mergeCell ref="C125:C127"/>
     <mergeCell ref="D125:D127"/>
     <mergeCell ref="A128:A130"/>
     <mergeCell ref="C128:C130"/>
     <mergeCell ref="D128:D130"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="D117:D120"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="D121:D124"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="main" display="https://chatgpt.com/ - main" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>

<commit_message>
dodaden broj na commit od pred merganje na main vo contactAdminReviews.
</commit_message>
<xml_diff>
--- a/Project-MRA/Project MRA.xlsx
+++ b/Project-MRA/Project MRA.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="828">
   <si>
     <t>Contact details</t>
   </si>
@@ -10017,6 +10017,9 @@
       </rPr>
       <t>reviews.html</t>
     </r>
+  </si>
+  <si>
+    <t>4f62d42</t>
   </si>
 </sst>
 </file>
@@ -14562,10 +14565,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G70"/>
+  <dimension ref="B2:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:D31"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -14573,67 +14576,70 @@
     <col min="1" max="16384" width="9.109375" style="42"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:15">
       <c r="B2" s="42" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:15">
       <c r="C3" s="42" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:15">
       <c r="D4" s="42" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:15">
       <c r="C5" s="42" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:15">
       <c r="C6" s="42" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:15">
       <c r="B8" s="42" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:15">
       <c r="C9" s="42" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:15">
       <c r="D10" s="42" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:15">
       <c r="C11" s="42" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
+      <c r="O11" s="42" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
       <c r="B13" s="42" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:15">
       <c r="C14" s="42" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:15">
       <c r="D15" s="42" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:15">
       <c r="C16" s="45" t="s">
         <v>816</v>
       </c>
@@ -17551,18 +17557,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="D128:D130"/>
     <mergeCell ref="A117:A120"/>
     <mergeCell ref="C117:C120"/>
     <mergeCell ref="D117:D120"/>
     <mergeCell ref="A121:A124"/>
     <mergeCell ref="C121:C124"/>
     <mergeCell ref="D121:D124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="A128:A130"/>
-    <mergeCell ref="C128:C130"/>
-    <mergeCell ref="D128:D130"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="main" display="https://chatgpt.com/ - main"/>

</xml_diff>